<commit_message>
Update Individual Time Sheet.xlsx
</commit_message>
<xml_diff>
--- a/Individual Time Sheet.xlsx
+++ b/Individual Time Sheet.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\GoogleDrive\study\2020\Semester 2\HIT 339\week 1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\GoogleDrive\study\2020\Semester 2\HIT 339\week 1\Week1 HelloWorldMVC\HIT339_Qingyuan_Zeng\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE532BCE-E3D0-41AF-A96A-60DCEAD5B53B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{721BF3C7-E89E-4DF0-856C-DBCCD90E67CA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9435" yWindow="1935" windowWidth="17085" windowHeight="12420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9945" yWindow="975" windowWidth="17085" windowHeight="12420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
   <si>
     <t>week1</t>
   </si>
@@ -126,12 +126,6 @@
     <t xml:space="preserve">1. Read "What is the MVC pattern?"
 2. Create new Github repo and folder 3. Install Visual Studio 2019 and .NET Core 3.1 SDK
 4. Create individul time sheet </t>
-  </si>
-  <si>
-    <t xml:space="preserve">1. Install SQL Express
-2. Install Resharper
-3. Install Source Tree
-</t>
   </si>
 </sst>
 </file>
@@ -221,8 +215,8 @@
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>6032</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>742951</xdr:rowOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>19051</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -524,7 +518,7 @@
   <dimension ref="A1:M21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -578,13 +572,11 @@
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="3" t="s">
-        <v>33</v>
-      </c>
+      <c r="B3" s="3"/>
     </row>
     <row r="4" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">

</xml_diff>